<commit_message>
Done: Payments and Links tables
</commit_message>
<xml_diff>
--- a/טבלאות db.xlsx
+++ b/טבלאות db.xlsx
@@ -1075,8 +1075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="G1:W27"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="I1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="M1" zoomScale="90" workbookViewId="0">
+      <selection activeCell="U9" sqref="U9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Done: Action Patterns tablegit add .
</commit_message>
<xml_diff>
--- a/טבלאות db.xlsx
+++ b/טבלאות db.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="68">
   <si>
     <t>id</t>
   </si>
@@ -225,13 +225,16 @@
   </si>
   <si>
     <t>אסתר</t>
+  </si>
+  <si>
+    <t>In Proccess</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -284,6 +287,13 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="177"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -360,7 +370,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -395,6 +405,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1064,8 +1075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="G1:W27"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="M1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="T6" sqref="T6"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="K1" zoomScale="90" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1090,6 +1101,12 @@
         <v>50</v>
       </c>
       <c r="I6" s="1"/>
+      <c r="N6" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="R6" s="17" t="s">
+        <v>64</v>
+      </c>
       <c r="T6" s="17" t="s">
         <v>64</v>
       </c>

</xml_diff>

<commit_message>
Done: Files table (:
</commit_message>
<xml_diff>
--- a/טבלאות db.xlsx
+++ b/טבלאות db.xlsx
@@ -1075,8 +1075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="G1:W27"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="K1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="M1" zoomScale="90" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1101,7 +1101,10 @@
         <v>50</v>
       </c>
       <c r="I6" s="1"/>
-      <c r="N6" s="20" t="s">
+      <c r="N6" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="P6" s="20" t="s">
         <v>67</v>
       </c>
       <c r="R6" s="17" t="s">
@@ -1172,9 +1175,7 @@
       <c r="L9" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="N9" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="N9" s="3"/>
       <c r="P9" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
Done: Actions table (;
</commit_message>
<xml_diff>
--- a/טבלאות db.xlsx
+++ b/טבלאות db.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="67">
   <si>
     <t>id</t>
   </si>
@@ -225,16 +225,13 @@
   </si>
   <si>
     <t>אסתר</t>
-  </si>
-  <si>
-    <t>In Proccess</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -287,13 +284,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="177"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -370,7 +360,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -405,7 +395,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1075,8 +1064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="G1:W27"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="M1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="M4" zoomScale="90" workbookViewId="0">
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1104,8 +1093,8 @@
       <c r="N6" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="P6" s="20" t="s">
-        <v>67</v>
+      <c r="P6" s="17" t="s">
+        <v>64</v>
       </c>
       <c r="R6" s="17" t="s">
         <v>64</v>

</xml_diff>